<commit_message>
sell furniture project + applying small updates on generator
</commit_message>
<xml_diff>
--- a/information.xlsx
+++ b/information.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lluis\Desktop\Projects\Portfolio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2D6E434-2C40-46AF-AD7B-457811420481}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D071B9FF-64B9-4DE1-8461-E5D273791FF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" firstSheet="2" activeTab="6" xr2:uid="{9CEA0154-E674-4F6E-9626-759C59FC0DAB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" firstSheet="2" activeTab="5" xr2:uid="{9CEA0154-E674-4F6E-9626-759C59FC0DAB}"/>
   </bookViews>
   <sheets>
     <sheet name="ABOUT" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="606" uniqueCount="475">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="615" uniqueCount="481">
   <si>
     <t>NAME</t>
   </si>
@@ -4384,6 +4384,24 @@
   </si>
   <si>
     <t>auto_portfolio_i.png</t>
+  </si>
+  <si>
+    <t>sell_furniture.png</t>
+  </si>
+  <si>
+    <t>June 2025</t>
+  </si>
+  <si>
+    <t>LINK|https://home-items-lluis.onrender.com/</t>
+  </si>
+  <si>
+    <t>Furniture Sale Showcase Website</t>
+  </si>
+  <si>
+    <t>sell_furniture_i.png</t>
+  </si>
+  <si>
+    <t>I created a small, responsive website to showcase furniture and items we planned to sell before moving out of an apartment. &lt;br/&gt; The site includes an image carousel for each item, item details like title and price, and a navigation system to browse through the collection. &lt;br/&gt; For privacy reasons, the images are not public, and the GitHub repository will remain private.</t>
   </si>
 </sst>
 </file>
@@ -5982,10 +6000,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8F62B72-F402-45A6-8AE4-4CD1EFC18BAE}">
-  <dimension ref="A1:I38"/>
+  <dimension ref="A1:I39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6031,222 +6049,222 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>459</v>
+        <v>478</v>
       </c>
       <c r="B2" t="s">
         <v>303</v>
       </c>
       <c r="C2" t="s">
-        <v>443</v>
+        <v>475</v>
       </c>
       <c r="D2" t="s">
-        <v>460</v>
+        <v>476</v>
       </c>
       <c r="E2" t="s">
-        <v>474</v>
+        <v>479</v>
       </c>
       <c r="F2" t="s">
-        <v>332</v>
+        <v>253</v>
       </c>
       <c r="G2" t="s">
-        <v>468</v>
+        <v>348</v>
       </c>
       <c r="H2" t="s">
-        <v>461</v>
+        <v>477</v>
       </c>
       <c r="I2" t="s">
-        <v>467</v>
+        <v>480</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>262</v>
+        <v>459</v>
       </c>
       <c r="B3" t="s">
-        <v>215</v>
+        <v>303</v>
       </c>
       <c r="C3" t="s">
-        <v>219</v>
+        <v>443</v>
       </c>
       <c r="D3" t="s">
-        <v>217</v>
+        <v>460</v>
       </c>
       <c r="E3" t="s">
-        <v>442</v>
+        <v>474</v>
       </c>
       <c r="F3" t="s">
         <v>332</v>
       </c>
       <c r="G3" t="s">
-        <v>271</v>
+        <v>468</v>
       </c>
       <c r="H3" t="s">
-        <v>412</v>
+        <v>461</v>
       </c>
       <c r="I3" t="s">
-        <v>301</v>
+        <v>467</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>302</v>
+        <v>262</v>
       </c>
       <c r="B4" t="s">
-        <v>303</v>
+        <v>215</v>
       </c>
       <c r="C4" t="s">
-        <v>341</v>
+        <v>219</v>
       </c>
       <c r="D4" t="s">
-        <v>339</v>
+        <v>217</v>
       </c>
       <c r="E4" t="s">
-        <v>341</v>
+        <v>442</v>
       </c>
       <c r="F4" t="s">
-        <v>253</v>
+        <v>332</v>
       </c>
       <c r="G4" t="s">
-        <v>342</v>
+        <v>271</v>
       </c>
       <c r="H4" t="s">
-        <v>421</v>
+        <v>412</v>
       </c>
       <c r="I4" t="s">
-        <v>340</v>
+        <v>301</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="B5" t="s">
         <v>303</v>
       </c>
       <c r="C5" t="s">
-        <v>347</v>
+        <v>341</v>
       </c>
       <c r="D5" t="s">
-        <v>346</v>
+        <v>339</v>
       </c>
       <c r="E5" t="s">
-        <v>347</v>
+        <v>341</v>
       </c>
       <c r="F5" t="s">
         <v>253</v>
       </c>
       <c r="G5" t="s">
-        <v>348</v>
+        <v>342</v>
       </c>
       <c r="H5" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="I5" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B6" t="s">
         <v>303</v>
       </c>
       <c r="C6" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="D6" t="s">
         <v>346</v>
       </c>
       <c r="E6" t="s">
-        <v>453</v>
+        <v>347</v>
       </c>
       <c r="F6" t="s">
-        <v>333</v>
+        <v>253</v>
       </c>
       <c r="G6" t="s">
         <v>348</v>
       </c>
-      <c r="H6" s="2" t="s">
-        <v>423</v>
+      <c r="H6" t="s">
+        <v>422</v>
       </c>
       <c r="I6" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>66</v>
+        <v>305</v>
       </c>
       <c r="B7" t="s">
         <v>303</v>
       </c>
       <c r="C7" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="D7" t="s">
-        <v>352</v>
+        <v>346</v>
       </c>
       <c r="E7" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="F7" t="s">
-        <v>253</v>
+        <v>333</v>
       </c>
       <c r="G7" t="s">
         <v>348</v>
       </c>
-      <c r="H7" t="s">
-        <v>424</v>
+      <c r="H7" s="2" t="s">
+        <v>423</v>
       </c>
       <c r="I7" t="s">
-        <v>437</v>
+        <v>349</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>306</v>
+        <v>66</v>
       </c>
       <c r="B8" t="s">
         <v>303</v>
       </c>
       <c r="C8" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="D8" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="E8" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="F8" t="s">
         <v>253</v>
       </c>
       <c r="G8" t="s">
-        <v>342</v>
+        <v>348</v>
       </c>
       <c r="H8" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="I8" t="s">
-        <v>355</v>
+        <v>437</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B9" t="s">
         <v>303</v>
       </c>
       <c r="C9" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="D9" t="s">
         <v>353</v>
       </c>
       <c r="E9" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="F9" t="s">
         <v>253</v>
@@ -6255,287 +6273,290 @@
         <v>342</v>
       </c>
       <c r="H9" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="I9" t="s">
-        <v>436</v>
+        <v>355</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B10" t="s">
         <v>303</v>
       </c>
       <c r="C10" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="D10" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="E10" t="s">
-        <v>358</v>
+        <v>456</v>
       </c>
       <c r="F10" t="s">
-        <v>333</v>
+        <v>253</v>
       </c>
       <c r="G10" t="s">
-        <v>359</v>
+        <v>342</v>
       </c>
       <c r="H10" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="I10" t="s">
-        <v>362</v>
+        <v>436</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B11" t="s">
-        <v>310</v>
+        <v>303</v>
       </c>
       <c r="C11" t="s">
-        <v>444</v>
+        <v>358</v>
       </c>
       <c r="D11" t="s">
-        <v>363</v>
+        <v>357</v>
+      </c>
+      <c r="E11" t="s">
+        <v>358</v>
       </c>
       <c r="F11" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="G11" t="s">
-        <v>364</v>
+        <v>359</v>
       </c>
       <c r="H11" t="s">
-        <v>413</v>
+        <v>427</v>
       </c>
       <c r="I11" t="s">
-        <v>438</v>
+        <v>362</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="B12" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="C12" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="D12" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
       <c r="F12" t="s">
-        <v>222</v>
+        <v>334</v>
       </c>
       <c r="G12" t="s">
-        <v>271</v>
+        <v>364</v>
       </c>
       <c r="H12" t="s">
-        <v>428</v>
+        <v>413</v>
       </c>
       <c r="I12" t="s">
-        <v>365</v>
+        <v>438</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>435</v>
+        <v>311</v>
       </c>
       <c r="B13" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C13" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="D13" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="F13" t="s">
-        <v>335</v>
+        <v>222</v>
       </c>
       <c r="G13" t="s">
         <v>271</v>
       </c>
       <c r="H13" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="I13" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>314</v>
+        <v>435</v>
       </c>
       <c r="B14" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="C14" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="D14" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="F14" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="G14" t="s">
-        <v>371</v>
+        <v>271</v>
       </c>
       <c r="H14" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="I14" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B15" t="s">
-        <v>303</v>
+        <v>315</v>
       </c>
       <c r="C15" t="s">
-        <v>443</v>
+        <v>447</v>
       </c>
       <c r="D15" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="F15" t="s">
-        <v>253</v>
+        <v>336</v>
       </c>
       <c r="G15" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="H15" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="I15" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B16" t="s">
         <v>303</v>
       </c>
       <c r="C16" t="s">
-        <v>441</v>
+        <v>443</v>
       </c>
       <c r="D16" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="F16" t="s">
-        <v>337</v>
+        <v>253</v>
       </c>
       <c r="G16" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="H16" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="I16" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B17" t="s">
-        <v>310</v>
+        <v>303</v>
       </c>
       <c r="C17" t="s">
-        <v>448</v>
+        <v>441</v>
       </c>
       <c r="D17" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="F17" t="s">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="G17" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="H17" t="s">
-        <v>419</v>
+        <v>432</v>
       </c>
       <c r="I17" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B18" t="s">
         <v>310</v>
       </c>
       <c r="C18" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D18" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="F18" t="s">
         <v>335</v>
       </c>
       <c r="G18" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="H18" t="s">
-        <v>414</v>
+        <v>419</v>
       </c>
       <c r="I18" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B19" t="s">
-        <v>321</v>
+        <v>310</v>
       </c>
       <c r="C19" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="D19" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="F19" t="s">
-        <v>222</v>
+        <v>335</v>
       </c>
       <c r="G19" t="s">
-        <v>271</v>
+        <v>383</v>
       </c>
       <c r="H19" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="I19" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B20" t="s">
-        <v>215</v>
+        <v>321</v>
       </c>
       <c r="C20" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="D20" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="F20" t="s">
         <v>222</v>
@@ -6544,176 +6565,199 @@
         <v>271</v>
       </c>
       <c r="H20" t="s">
-        <v>458</v>
+        <v>415</v>
       </c>
       <c r="I20" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B21" t="s">
-        <v>324</v>
+        <v>215</v>
       </c>
       <c r="C21" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D21" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="F21" t="s">
         <v>222</v>
       </c>
       <c r="G21" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
       <c r="H21" t="s">
-        <v>416</v>
+        <v>458</v>
       </c>
       <c r="I21" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="B22" t="s">
-        <v>303</v>
+        <v>324</v>
       </c>
       <c r="C22" t="s">
-        <v>391</v>
+        <v>452</v>
       </c>
       <c r="D22" t="s">
-        <v>392</v>
-      </c>
-      <c r="E22" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="F22" t="s">
-        <v>253</v>
+        <v>222</v>
       </c>
       <c r="G22" t="s">
-        <v>393</v>
+        <v>276</v>
       </c>
       <c r="H22" t="s">
-        <v>433</v>
+        <v>416</v>
       </c>
       <c r="I22" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B23" t="s">
         <v>303</v>
       </c>
       <c r="C23" t="s">
-        <v>440</v>
+        <v>391</v>
       </c>
       <c r="D23" t="s">
-        <v>398</v>
+        <v>392</v>
+      </c>
+      <c r="E23" t="s">
+        <v>391</v>
       </c>
       <c r="F23" t="s">
         <v>253</v>
       </c>
       <c r="G23" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="H23" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="I23" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B24" t="s">
-        <v>310</v>
+        <v>303</v>
       </c>
       <c r="C24" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="D24" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="F24" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="G24" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
       <c r="H24" t="s">
-        <v>420</v>
+        <v>434</v>
       </c>
       <c r="I24" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B25" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="C25" t="s">
-        <v>403</v>
+        <v>439</v>
       </c>
       <c r="D25" t="s">
-        <v>402</v>
-      </c>
-      <c r="E25" t="s">
-        <v>403</v>
+        <v>397</v>
       </c>
       <c r="F25" t="s">
         <v>252</v>
       </c>
       <c r="G25" t="s">
-        <v>271</v>
+        <v>399</v>
       </c>
       <c r="H25" t="s">
-        <v>417</v>
+        <v>420</v>
       </c>
       <c r="I25" t="s">
-        <v>401</v>
+        <v>396</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
+        <v>328</v>
+      </c>
+      <c r="B26" t="s">
+        <v>313</v>
+      </c>
+      <c r="C26" t="s">
+        <v>403</v>
+      </c>
+      <c r="D26" t="s">
+        <v>402</v>
+      </c>
+      <c r="E26" t="s">
+        <v>403</v>
+      </c>
+      <c r="F26" t="s">
+        <v>252</v>
+      </c>
+      <c r="G26" t="s">
+        <v>271</v>
+      </c>
+      <c r="H26" t="s">
+        <v>417</v>
+      </c>
+      <c r="I26" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>330</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B27" t="s">
         <v>329</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C27" t="s">
         <v>457</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D27" t="s">
         <v>404</v>
       </c>
-      <c r="F26" t="s">
+      <c r="F27" t="s">
         <v>338</v>
       </c>
-      <c r="G26" t="s">
+      <c r="G27" t="s">
         <v>405</v>
       </c>
-      <c r="H26" t="s">
+      <c r="H27" t="s">
         <v>418</v>
       </c>
-      <c r="I26" t="s">
+      <c r="I27" t="s">
         <v>406</v>
       </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E28" s="1"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E29" s="1"/>
@@ -6744,11 +6788,14 @@
     </row>
     <row r="38" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E38" s="1"/>
+    </row>
+    <row r="39" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E39" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="H6" r:id="rId1" display="https://github.com/lluisg/fontvisualizer" xr:uid="{4E0AF6C4-0111-4171-962F-87619946D9FF}"/>
+    <hyperlink ref="H7" r:id="rId1" display="https://github.com/lluisg/fontvisualizer" xr:uid="{4E0AF6C4-0111-4171-962F-87619946D9FF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
@@ -6759,7 +6806,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05BCBF17-B846-480B-A437-F9769858B36E}">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>

</xml_diff>